<commit_message>
Change active to passive voice
</commit_message>
<xml_diff>
--- a/Paper/graphs.xlsx
+++ b/Paper/graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\MeltdownAttack\Paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399AF6DF-367C-4B67-8026-1A9732210CAB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2AA8F7D-03A3-4781-9BC5-BC7307D9AB17}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7520" activeTab="2" xr2:uid="{A4E5F0FF-BC91-4E7C-BFFE-A6EC0E972353}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Success Rate (%)</t>
   </si>
@@ -1285,37 +1285,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -4515,7 +4485,7 @@
   <dimension ref="B4:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:C26"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>